<commit_message>
added the orginal csv
</commit_message>
<xml_diff>
--- a/data/lossofsale_sg_chavakkad.xlsx
+++ b/data/lossofsale_sg_chavakkad.xlsx
@@ -206,12 +206,12 @@
     <col min="3" max="3" width="17.55" customWidth="1"/>
     <col min="4" max="4" width="13.5" customWidth="1"/>
     <col min="5" max="5" width="17.55" customWidth="1"/>
-    <col min="6" max="6" width="22.950000000000003" customWidth="1"/>
+    <col min="6" max="6" width="10.8" customWidth="1"/>
     <col min="7" max="7" width="8.100000000000001" customWidth="1"/>
     <col min="8" max="8" width="32.400000000000006" customWidth="1"/>
-    <col min="9" max="9" width="36.45" customWidth="1"/>
+    <col min="9" max="9" width="37.800000000000004" customWidth="1"/>
     <col min="10" max="10" width="16.200000000000003" customWidth="1"/>
-    <col min="11" max="11" width="49.95" customWidth="1"/>
+    <col min="11" max="11" width="29.700000000000003" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -284,25 +284,25 @@
       </c>
       <c t="inlineStr" r="B3">
         <is>
-          <t xml:space="preserve">01-12-2025</t>
+          <t xml:space="preserve">16-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C3">
         <is>
-          <t xml:space="preserve">thanseer</t>
+          <t xml:space="preserve">Abdul razzaq</t>
         </is>
       </c>
       <c r="D3" s="65">
-        <v>9947454748</v>
+        <v>9746697775</v>
       </c>
       <c t="inlineStr" r="E3">
         <is>
-          <t xml:space="preserve">07-12-2025</t>
+          <t xml:space="preserve">17-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="F3">
         <is>
-          <t xml:space="preserve">MUHAMMED ASLAM VB</t>
+          <t xml:space="preserve">MAHESH C</t>
         </is>
       </c>
       <c t="inlineStr" r="G3">
@@ -327,7 +327,7 @@
       </c>
       <c t="inlineStr" r="K3">
         <is>
-          <t xml:space="preserve">.</t>
+          <t xml:space="preserve">BIG SIZE</t>
         </is>
       </c>
     </row>
@@ -337,20 +337,20 @@
       </c>
       <c t="inlineStr" r="B4">
         <is>
-          <t xml:space="preserve">01-12-2025</t>
+          <t xml:space="preserve">16-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C4">
         <is>
-          <t xml:space="preserve">naji</t>
+          <t xml:space="preserve">fasil</t>
         </is>
       </c>
       <c r="D4" s="65">
-        <v>9074020097</v>
+        <v>9961122822</v>
       </c>
       <c t="inlineStr" r="E4">
         <is>
-          <t xml:space="preserve">31-12-2025</t>
+          <t xml:space="preserve">25-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="F4">
@@ -370,17 +370,17 @@
       </c>
       <c t="inlineStr" r="I4">
         <is>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
+        </is>
+      </c>
+      <c t="inlineStr" r="J4">
+        <is>
           <t xml:space="preserve">-</t>
         </is>
       </c>
-      <c t="inlineStr" r="J4">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
       <c t="inlineStr" r="K4">
         <is>
-          <t xml:space="preserve">BULK BOOKING KURTA COUSINS ARE ABROAD</t>
+          <t xml:space="preserve">GROOM IS NOT AVIALABLE</t>
         </is>
       </c>
     </row>
@@ -390,25 +390,25 @@
       </c>
       <c t="inlineStr" r="B5">
         <is>
-          <t xml:space="preserve">02-12-2025</t>
+          <t xml:space="preserve">16-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C5">
         <is>
-          <t xml:space="preserve">shamil</t>
+          <t xml:space="preserve">shaheer</t>
         </is>
       </c>
       <c r="D5" s="65">
-        <v>8593988205</v>
+        <v>7559857541</v>
       </c>
       <c t="inlineStr" r="E5">
         <is>
-          <t xml:space="preserve">11-01-2026</t>
+          <t xml:space="preserve">28-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="F5">
         <is>
-          <t xml:space="preserve">MUHAMMED ASLAM VB</t>
+          <t xml:space="preserve">MAHESH C</t>
         </is>
       </c>
       <c t="inlineStr" r="G5">
@@ -423,17 +423,12 @@
       </c>
       <c t="inlineStr" r="I5">
         <is>
-          <t xml:space="preserve">ENQUIRY WITHOUT TRIAL</t>
+          <t xml:space="preserve">ENQUIRY WITHOUT BRIDE/FAMILY</t>
         </is>
       </c>
       <c t="inlineStr" r="J5">
         <is>
           <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="K5">
-        <is>
-          <t xml:space="preserve">.</t>
         </is>
       </c>
     </row>
@@ -443,25 +438,25 @@
       </c>
       <c t="inlineStr" r="B6">
         <is>
-          <t xml:space="preserve">02-12-2025</t>
+          <t xml:space="preserve">16-12-2025</t>
         </is>
       </c>
       <c t="inlineStr" r="C6">
         <is>
-          <t xml:space="preserve">jasim</t>
+          <t xml:space="preserve">ajmal</t>
         </is>
       </c>
       <c r="D6" s="65">
-        <v>9562729920</v>
+        <v>8139089882</v>
       </c>
       <c t="inlineStr" r="E6">
         <is>
-          <t xml:space="preserve">14-12-2025</t>
+          <t xml:space="preserve">14-01-2026</t>
         </is>
       </c>
       <c t="inlineStr" r="F6">
         <is>
-          <t xml:space="preserve">RASAL</t>
+          <t xml:space="preserve">MAHESH C</t>
         </is>
       </c>
       <c t="inlineStr" r="G6">
@@ -471,12 +466,12 @@
       </c>
       <c t="inlineStr" r="H6">
         <is>
-          <t xml:space="preserve">PRODUCT</t>
+          <t xml:space="preserve">CUSTOMER INTERNAL ISSUES</t>
         </is>
       </c>
       <c t="inlineStr" r="I6">
         <is>
-          <t xml:space="preserve">PRODUCT NOT AVAILABLE</t>
+          <t xml:space="preserve">BUDGET RESTRICTIONS</t>
         </is>
       </c>
       <c t="inlineStr" r="J6">
@@ -486,161 +481,7 @@
       </c>
       <c t="inlineStr" r="K6">
         <is>
-          <t xml:space="preserve">trending armani kurta</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="65">
-        <v>5</v>
-      </c>
-      <c t="inlineStr" r="B7">
-        <is>
-          <t xml:space="preserve">02-12-2025</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="C7">
-        <is>
-          <t xml:space="preserve">sreeraj</t>
-        </is>
-      </c>
-      <c r="D7" s="65">
-        <v>9746497472</v>
-      </c>
-      <c t="inlineStr" r="E7">
-        <is>
-          <t xml:space="preserve">07-12-2025</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F7">
-        <is>
-          <t xml:space="preserve">MUHAMMED ASLAM VB</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="G7">
-        <is>
-          <t xml:space="preserve">Loss</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="H7">
-        <is>
-          <t xml:space="preserve">CUSTOMER INTERNAL ISSUES</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="I7">
-        <is>
-          <t xml:space="preserve">FAMILY DISAPPROVEL</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="J7">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="K7">
-        <is>
-          <t xml:space="preserve">.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="65">
-        <v>6</v>
-      </c>
-      <c t="inlineStr" r="B8">
-        <is>
-          <t xml:space="preserve">03-12-2025</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="C8">
-        <is>
-          <t xml:space="preserve">sana</t>
-        </is>
-      </c>
-      <c r="D8" s="65">
-        <v>9633445624</v>
-      </c>
-      <c t="inlineStr" r="E8">
-        <is>
-          <t xml:space="preserve">21-12-2025</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F8">
-        <is>
-          <t xml:space="preserve">MUHAMMED ASLAM VB</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="G8">
-        <is>
-          <t xml:space="preserve">Loss</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="H8">
-        <is>
-          <t xml:space="preserve">ENQUIRY</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="I8">
-        <is>
-          <t xml:space="preserve">Enquiry for Relative/Friend</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="J8">
-        <is>
-          <t xml:space="preserve">-</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="K8">
-        <is>
-          <t xml:space="preserve">groom is abroad</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="65">
-        <v>7</v>
-      </c>
-      <c t="inlineStr" r="B9">
-        <is>
-          <t xml:space="preserve">03-12-2025</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="C9">
-        <is>
-          <t xml:space="preserve">Abishek</t>
-        </is>
-      </c>
-      <c r="D9" s="65">
-        <v>811390232</v>
-      </c>
-      <c t="inlineStr" r="E9">
-        <is>
-          <t xml:space="preserve">20-12-2025</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="F9">
-        <is>
-          <t xml:space="preserve">RASAL</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="G9">
-        <is>
-          <t xml:space="preserve">Loss</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="H9">
-        <is>
-          <t xml:space="preserve">CUSTOMER INTERNAL ISSUES</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="I9">
-        <is>
-          <t xml:space="preserve">FAMILY DISAPPROVEL</t>
-        </is>
-      </c>
-      <c t="inlineStr" r="J9">
-        <is>
-          <t xml:space="preserve">-</t>
+          <t xml:space="preserve">CONFIRM TMRW</t>
         </is>
       </c>
     </row>

</xml_diff>